<commit_message>
funguje dynamicky vypocet mandatu
</commit_message>
<xml_diff>
--- a/volebni_analyza_2025_finalni_opravena.xlsx
+++ b/volebni_analyza_2025_finalni_opravena.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pridelene_mandaty" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Analyza_hlasu" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -899,197 +898,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Strana</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Celkem hlasů</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Hlasy použité v 1. skrutiniu</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Hlasy použité v 2. skrutiniu</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Přeteklé / nevyužité hlasy</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>SPD</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>437611</v>
-      </c>
-      <c r="C2" t="n">
-        <v>300958</v>
-      </c>
-      <c r="D2" t="n">
-        <v>137360</v>
-      </c>
-      <c r="E2" t="n">
-        <v>-707</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>SPOLU</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>1313346</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1150983</v>
-      </c>
-      <c r="D3" t="n">
-        <v>137360</v>
-      </c>
-      <c r="E3" t="n">
-        <v>25003</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Piráti</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>504537</v>
-      </c>
-      <c r="C4" t="n">
-        <v>371190</v>
-      </c>
-      <c r="D4" t="n">
-        <v>137360</v>
-      </c>
-      <c r="E4" t="n">
-        <v>-4013</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>AUTO</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>380601</v>
-      </c>
-      <c r="C5" t="n">
-        <v>252794</v>
-      </c>
-      <c r="D5" t="n">
-        <v>137360</v>
-      </c>
-      <c r="E5" t="n">
-        <v>-9553</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>ANO</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>1940507</v>
-      </c>
-      <c r="C6" t="n">
-        <v>1776334</v>
-      </c>
-      <c r="D6" t="n">
-        <v>137360</v>
-      </c>
-      <c r="E6" t="n">
-        <v>26813</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>STAN</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>631512</v>
-      </c>
-      <c r="C7" t="n">
-        <v>463018</v>
-      </c>
-      <c r="D7" t="n">
-        <v>137360</v>
-      </c>
-      <c r="E7" t="n">
-        <v>31134</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr"/>
-      <c r="B8" t="n">
-        <v>5208114</v>
-      </c>
-      <c r="C8" t="n">
-        <v>4315277</v>
-      </c>
-      <c r="D8" t="n">
-        <v>824160</v>
-      </c>
-      <c r="E8" t="n">
-        <v>68677</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr"/>
-      <c r="B9" t="n">
-        <v>413603</v>
-      </c>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="n">
-        <v>5621717</v>
-      </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>